<commit_message>
Inclusao de lib nltk na wordcloud
</commit_message>
<xml_diff>
--- a/palavras_chave.xlsx
+++ b/palavras_chave.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreluiz/Documents/projetos/analisador-audio-texto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andrelmr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81530D30-9D1D-E34B-AB5B-EF2FEB93074B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB09961-2439-44DE-9313-00F2EE3E2AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{4A322859-7E29-49B7-A160-5D7FA108ACE1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4A322859-7E29-49B7-A160-5D7FA108ACE1}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,42 +34,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Transferência</t>
-  </si>
-  <si>
-    <t>Depósito</t>
-  </si>
-  <si>
-    <t>Contrato</t>
-  </si>
-  <si>
-    <t>Dossie</t>
-  </si>
-  <si>
-    <t>Caixinha</t>
-  </si>
-  <si>
-    <t>Gerir</t>
-  </si>
-  <si>
-    <t>Acordo</t>
-  </si>
-  <si>
-    <t>Termo</t>
-  </si>
-  <si>
-    <t>Jesus</t>
-  </si>
-  <si>
-    <t>família</t>
-  </si>
-  <si>
-    <t>jesus abençoado</t>
-  </si>
-  <si>
-    <t>mensagem</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>porã</t>
+  </si>
+  <si>
+    <t>termo</t>
+  </si>
+  <si>
+    <t>gerir</t>
+  </si>
+  <si>
+    <t>transferência</t>
+  </si>
+  <si>
+    <t>depósito</t>
+  </si>
+  <si>
+    <t>contrato</t>
+  </si>
+  <si>
+    <t>dossiê</t>
+  </si>
+  <si>
+    <t>caixinha</t>
+  </si>
+  <si>
+    <t>acordo</t>
+  </si>
+  <si>
+    <t>dinheiro</t>
+  </si>
+  <si>
+    <t>propina</t>
+  </si>
+  <si>
+    <t>café</t>
+  </si>
+  <si>
+    <t>cafezinho</t>
+  </si>
+  <si>
+    <t>prefeito</t>
+  </si>
+  <si>
+    <t>governador</t>
+  </si>
+  <si>
+    <t>deputado</t>
+  </si>
+  <si>
+    <t>patrão</t>
   </si>
 </sst>
 </file>
@@ -429,75 +444,100 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A406B85-2F1A-4C28-8DE1-5C78F8BD1470}">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="222" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.1640625" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>